<commit_message>
use can except some sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/SmokeTests.xlsx
+++ b/src/test/resources/SmokeTests.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="820" windowWidth="22460" windowHeight="14280"/>
+    <workbookView xWindow="420" yWindow="820" windowWidth="22460" windowHeight="14280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SmokeTest" sheetId="5" r:id="rId1"/>
+    <sheet name="DoNotConsider" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="65">
   <si>
     <t>Student Name</t>
   </si>
@@ -231,7 +232,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +267,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -315,7 +324,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
@@ -367,13 +376,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -415,6 +428,10 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Loop" xfId="4"/>
     <cellStyle name="Loop Parameter" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1338,4 +1355,139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>